<commit_message>
refactor of modelling and mapping flows to adopt 'Namespace' as top-object and relegate 'Domain' to more fluid definition
</commit_message>
<xml_diff>
--- a/src/models/serialisation_templates.xlsx
+++ b/src/models/serialisation_templates.xlsx
@@ -21,18 +21,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t xml:space="preserve">Sequence</t>
   </si>
   <si>
+    <t xml:space="preserve">Namespace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NamespaceDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ModelDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ModelType</t>
+  </si>
+  <si>
     <t xml:space="preserve">Domain</t>
   </si>
   <si>
-    <t xml:space="preserve">Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModelType</t>
+    <t xml:space="preserve">DomainDescription</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFE8F2A1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sub</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFE8F2A1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Domain</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Class</t>
@@ -50,12 +85,6 @@
     <t xml:space="preserve">DataType</t>
   </si>
   <si>
-    <t xml:space="preserve">Context</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SubContext</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nulls</t>
   </si>
   <si>
@@ -65,6 +94,9 @@
     <t xml:space="preserve">Relationship</t>
   </si>
   <si>
+    <t xml:space="preserve">FromModel</t>
+  </si>
+  <si>
     <t xml:space="preserve">FromClass</t>
   </si>
   <si>
@@ -74,6 +106,9 @@
     <t xml:space="preserve">FromCardinality</t>
   </si>
   <si>
+    <t xml:space="preserve">ToModel</t>
+  </si>
+  <si>
     <t xml:space="preserve">ToClass</t>
   </si>
   <si>
@@ -86,7 +121,7 @@
     <t xml:space="preserve">Mapping</t>
   </si>
   <si>
-    <t xml:space="preserve">SourceDomain</t>
+    <t xml:space="preserve">SourceNamespace</t>
   </si>
   <si>
     <t xml:space="preserve">SourceModel</t>
@@ -98,7 +133,7 @@
     <t xml:space="preserve">SourceAttribute</t>
   </si>
   <si>
-    <t xml:space="preserve">TargetDomain</t>
+    <t xml:space="preserve">TargetNamespace</t>
   </si>
   <si>
     <t xml:space="preserve">TargetModel</t>
@@ -120,7 +155,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -149,6 +184,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFE8F2A1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -213,7 +255,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -222,7 +264,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -303,23 +349,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q12" activeCellId="0" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="5.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="14" style="0" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="10" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="5.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="17" style="0" width="20.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -341,10 +391,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -382,6 +432,21 @@
       </c>
       <c r="T1" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -400,51 +465,56 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="4" style="0" width="17.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>29</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated DMEAR to include new Domain and DomainEvent concepts
</commit_message>
<xml_diff>
--- a/src/models/serialisation_templates.xlsx
+++ b/src/models/serialisation_templates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="DMEAR" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,6 +32,15 @@
     <t xml:space="preserve">NamespaceDescription</t>
   </si>
   <si>
+    <t xml:space="preserve">Domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomainDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SubDomain</t>
+  </si>
+  <si>
     <t xml:space="preserve">Model</t>
   </si>
   <si>
@@ -39,35 +48,6 @@
   </si>
   <si>
     <t xml:space="preserve">ModelType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Domain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DomainDescription</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FFE8F2A1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Sub</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FFE8F2A1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Domain</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Class</t>
@@ -155,7 +135,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -184,13 +164,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFE8F2A1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -255,7 +228,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -264,11 +237,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -351,11 +320,11 @@
   </sheetPr>
   <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q12" activeCellId="0" sqref="Q12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.59"/>
@@ -363,10 +332,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="10" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="5.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="17" style="0" width="20.7"/>
@@ -391,10 +361,10 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -467,11 +437,11 @@
   </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.86"/>
@@ -480,40 +450,40 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DMEAR (soon to be DMCAR) model changes and serialization updates, including new serialization_template.xlsx template
</commit_message>
<xml_diff>
--- a/src/models/serialisation_templates.xlsx
+++ b/src/models/serialisation_templates.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="DMEAR" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="DMCAR" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Mapping" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -21,47 +21,80 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+  <si>
+    <t xml:space="preserve">Namespace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NamespaceLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NamespaceDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomainLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomainDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ParentDomain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomainEvent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomainEventLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomainEventDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomainParticipant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomainParticipantLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DomainParticipantDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ModelLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ModelDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ModelType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClassLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClassDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AttributeLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AttributeDescription</t>
+  </si>
   <si>
     <t xml:space="preserve">Sequence</t>
   </si>
   <si>
-    <t xml:space="preserve">Namespace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NamespaceDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Domain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DomainDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SubDomain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModelDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModelType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ClassDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attribute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AttributeDescription</t>
-  </si>
-  <si>
     <t xml:space="preserve">DataType</t>
   </si>
   <si>
@@ -74,7 +107,13 @@
     <t xml:space="preserve">Relationship</t>
   </si>
   <si>
-    <t xml:space="preserve">FromModel</t>
+    <t xml:space="preserve">RelationshipLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RelationshipDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FromNamespace</t>
   </si>
   <si>
     <t xml:space="preserve">FromClass</t>
@@ -86,7 +125,27 @@
     <t xml:space="preserve">FromCardinality</t>
   </si>
   <si>
-    <t xml:space="preserve">ToModel</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">To</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Namespace</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">ToClass</t>
@@ -135,7 +194,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -159,22 +218,35 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFE8F2A1"/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFDEE6EF"/>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,14 +255,56 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF069A2E"/>
-        <bgColor rgb="FF339966"/>
+        <fgColor rgb="FF418AFF"/>
+        <bgColor rgb="FF3465A4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA23EFF"/>
+        <bgColor rgb="FFD83DFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD83DFF"/>
+        <bgColor rgb="FFA23EFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF79FC"/>
+        <bgColor rgb="FFCC99FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFBF00"/>
+        <bgColor rgb="FFFF8000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF3465A4"/>
-        <bgColor rgb="FF3366FF"/>
+        <bgColor rgb="FF0066CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -228,7 +342,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -237,7 +351,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -258,10 +408,10 @@
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFD83DFF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF069A2E"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
@@ -269,9 +419,9 @@
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFA23EFF"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFDEE6EF"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -287,16 +437,16 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFE8F2A1"/>
+      <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFF79FC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF418AFF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFFBF00"/>
+      <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF3465A4"/>
       <rgbColor rgb="FF969696"/>
@@ -318,31 +468,51 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:AMJ1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB14" activeCellId="0" sqref="AB14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="10" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="5.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="17" style="0" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="33.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="20.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="0" width="22.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="6.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="6.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="19.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="10.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="15.46"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -352,72 +522,112 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="Z1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AMJ1" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -438,53 +648,50 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="4" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="4" style="0" width="22.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>34</v>
+      <c r="C1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added sizing heights on visualisations
</commit_message>
<xml_diff>
--- a/src/models/serialisation_templates.xlsx
+++ b/src/models/serialisation_templates.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DMCAR" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Mapping" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Requirement" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t xml:space="preserve">Namespace</t>
   </si>
@@ -168,6 +169,24 @@
   </si>
   <si>
     <t xml:space="preserve">Translation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PrimaryStakeholder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PrimaryStakeholderDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RequirementId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
   </si>
 </sst>
 </file>
@@ -442,18 +461,18 @@
   </sheetPr>
   <dimension ref="A1:AM1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE2" activeCellId="0" sqref="AE2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.71"/>
@@ -472,7 +491,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="14.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="0" width="19.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="13.1"/>
@@ -622,10 +641,10 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="4" style="0" width="22.36"/>
   </cols>
@@ -666,6 +685,59 @@
       </c>
       <c r="L1" s="10" t="s">
         <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.26"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>